<commit_message>
output table test fr paddleOCR
</commit_message>
<xml_diff>
--- a/main_script/output/table_0.xlsx
+++ b/main_script/output/table_0.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>1.600 GHz</t>
-  </si>
-  <si>
-    <t>16.369 4B]</t>
-  </si>
-  <si>
-    <t>k|</t>
+    <t>1.500 GHz</t>
+  </si>
+  <si>
+    <t>15.369 dB</t>
+  </si>
+  <si>
+    <t>9694.433 K</t>
   </si>
   <si>
     <t>15.584 dB</t>
@@ -34,23 +34,22 @@
     <t>13.778 dB</t>
   </si>
   <si>
-    <t>6632.240
-K</t>
-  </si>
-  <si>
-    <t>1.260 dB</t>
+    <t>6632.240 K</t>
+  </si>
+  <si>
+    <t>-15.260 dB</t>
   </si>
   <si>
     <t>2.500 GHz</t>
   </si>
   <si>
-    <t>14.638 dB</t>
-  </si>
-  <si>
-    <t>7954.975 K|</t>
-  </si>
-  <si>
-    <t>16.569 dB</t>
+    <t>14.538 dB</t>
+  </si>
+  <si>
+    <t>7954.975 K</t>
+  </si>
+  <si>
+    <t>-15.569 d8</t>
   </si>
   <si>
     <t>3.000 GHz</t>
@@ -62,32 +61,31 @@
     <t>8165.911 K</t>
   </si>
   <si>
-    <t>16.339 dB</t>
-  </si>
-  <si>
-    <t>3.800 GH
-Zz</t>
-  </si>
-  <si>
-    <t>15,802 dB</t>
-  </si>
-  <si>
-    <t>10740.832</t>
-  </si>
-  <si>
-    <t>15.978 dB</t>
-  </si>
-  <si>
-    <t>4,000 GHz</t>
+    <t>-15.339 dB</t>
+  </si>
+  <si>
+    <t>3.500 GHz</t>
+  </si>
+  <si>
+    <t>15.802 dB</t>
+  </si>
+  <si>
+    <t>10740.832 Kj</t>
+  </si>
+  <si>
+    <t>-15.978 dB</t>
+  </si>
+  <si>
+    <t>4.000 GHz</t>
   </si>
   <si>
     <t>15.510 dB</t>
   </si>
   <si>
-    <t>kK</t>
-  </si>
-  <si>
-    <t>15.796 dB</t>
+    <t>10023.732 K</t>
+  </si>
+  <si>
+    <t>-15.796 dB</t>
   </si>
 </sst>
 </file>
@@ -444,9 +442,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>